<commit_message>
a lot of changes, till monday
</commit_message>
<xml_diff>
--- a/genetic algorithm results.xlsx
+++ b/genetic algorithm results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-smaalumi\Desktop\AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD8A0CD-3EF3-4C65-B021-93680D23197F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9FC309-072B-45ED-935D-791A181C0095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,20 +671,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="2" max="2" width="90.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="171.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="163.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="254.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="90.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="171.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="163.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="254.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -702,7 +702,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>4</v>
       </c>
@@ -719,7 +719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>6</v>
       </c>
@@ -736,7 +736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>8</v>
       </c>
@@ -753,7 +753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>10</v>
       </c>
@@ -770,7 +770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>12</v>
       </c>
@@ -787,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>14</v>
       </c>
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>16</v>
       </c>
@@ -821,7 +821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>18</v>
       </c>
@@ -838,7 +838,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -855,7 +855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>22</v>
       </c>
@@ -872,7 +872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>24</v>
       </c>
@@ -889,7 +889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>26</v>
       </c>
@@ -906,7 +906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>28</v>
       </c>
@@ -923,7 +923,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>30</v>
       </c>
@@ -940,7 +940,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>32</v>
       </c>

</xml_diff>